<commit_message>
ext data for phyto tests, remove ems ext data
</commit_message>
<xml_diff>
--- a/inst/extdata/phyto/phyto1.xlsx
+++ b/inst/extdata/phyto/phyto1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/evanamies-galonski/Code/nrp/nrp/inst/extdata/phyto/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0DD0986-A1F9-A048-AE87-D9042EE29B3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFF6C300-B091-204E-92EB-970F799E4C0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="760" windowWidth="23900" windowHeight="14540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="26">
   <si>
     <t>Samp_Date</t>
   </si>
@@ -55,21 +55,9 @@
     <t>0-20M</t>
   </si>
   <si>
-    <t>Chryso- &amp; Cryptophyte</t>
-  </si>
-  <si>
-    <t>Flagellates</t>
-  </si>
-  <si>
     <t>E</t>
   </si>
   <si>
-    <t>Bacillariophyte</t>
-  </si>
-  <si>
-    <t>Diatoms</t>
-  </si>
-  <si>
     <t>Dinophyte</t>
   </si>
   <si>
@@ -82,12 +70,6 @@
     <t>Blue-greens</t>
   </si>
   <si>
-    <t>Synechococcus sp. (rod)</t>
-  </si>
-  <si>
-    <t>Synechococcus sp. (coccoid)</t>
-  </si>
-  <si>
     <t>Merismopedia sp. (cells)</t>
   </si>
   <si>
@@ -104,33 +86,6 @@
   </si>
   <si>
     <t>Gymnodinium sp. (medium)</t>
-  </si>
-  <si>
-    <t>Cyclotella sp.</t>
-  </si>
-  <si>
-    <t>Ochromonas sp.</t>
-  </si>
-  <si>
-    <t>Fragilaria crotonensis</t>
-  </si>
-  <si>
-    <t>I</t>
-  </si>
-  <si>
-    <t>Chroomonas acuta</t>
-  </si>
-  <si>
-    <t>Synedra ulna</t>
-  </si>
-  <si>
-    <t>Chrysococcus</t>
-  </si>
-  <si>
-    <t>Synedra acus var. angustissima</t>
-  </si>
-  <si>
-    <t>AR-4</t>
   </si>
   <si>
     <t>AR-5</t>
@@ -551,8 +506,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J179"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A163" workbookViewId="0">
-      <selection activeCell="A179" sqref="A17:J179"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K18" sqref="A9:K18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -592,10 +547,10 @@
         <v>6</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>39</v>
+        <v>24</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="J1" s="2" t="s">
         <v>7</v>
@@ -609,25 +564,28 @@
         <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>35</v>
+        <v>21</v>
       </c>
       <c r="D2" t="s">
         <v>9</v>
       </c>
       <c r="E2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2" s="5">
+        <v>2341.5652173912999</v>
+      </c>
+      <c r="I2" s="6">
+        <v>7.0246956521739104E-3</v>
+      </c>
+      <c r="J2" t="s">
         <v>10</v>
-      </c>
-      <c r="F2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G2" t="s">
-        <v>33</v>
-      </c>
-      <c r="H2" s="5">
-        <v>24.3913043478261</v>
-      </c>
-      <c r="I2" s="6">
-        <v>1.82934782608696E-3</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
@@ -638,28 +596,28 @@
         <v>8</v>
       </c>
       <c r="C3" t="s">
-        <v>35</v>
+        <v>21</v>
       </c>
       <c r="D3" t="s">
         <v>9</v>
       </c>
       <c r="E3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G3" t="s">
+        <v>18</v>
+      </c>
+      <c r="H3" s="5">
+        <v>48.7826086956522</v>
+      </c>
+      <c r="I3" s="6">
+        <v>2.4391304347826099E-3</v>
+      </c>
+      <c r="J3" t="s">
         <v>10</v>
-      </c>
-      <c r="F3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G3" t="s">
-        <v>31</v>
-      </c>
-      <c r="H3" s="5">
-        <v>121.95652173913</v>
-      </c>
-      <c r="I3" s="6">
-        <v>6.0978260869565199E-3</v>
-      </c>
-      <c r="J3" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
@@ -670,28 +628,28 @@
         <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>35</v>
+        <v>21</v>
       </c>
       <c r="D4" t="s">
         <v>9</v>
       </c>
       <c r="E4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F4" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="G4" t="s">
-        <v>32</v>
+        <v>19</v>
       </c>
       <c r="H4" s="5">
-        <v>170.73913043478299</v>
+        <v>48.7826086956522</v>
       </c>
       <c r="I4" s="6">
-        <v>5.1221739130434797E-2</v>
+        <v>9.7565217391304294E-3</v>
       </c>
       <c r="J4" t="s">
-        <v>30</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
@@ -702,28 +660,25 @@
         <v>8</v>
       </c>
       <c r="C5" t="s">
-        <v>35</v>
+        <v>21</v>
       </c>
       <c r="D5" t="s">
         <v>9</v>
       </c>
       <c r="E5" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F5" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="G5" t="s">
-        <v>34</v>
+        <v>20</v>
       </c>
       <c r="H5" s="5">
-        <v>48.7826086956522</v>
+        <v>73.173913043478294</v>
       </c>
       <c r="I5" s="6">
-        <v>7.3173913043478303E-3</v>
-      </c>
-      <c r="J5" t="s">
-        <v>30</v>
+        <v>2.92695652173913E-2</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
@@ -734,340 +689,59 @@
         <v>8</v>
       </c>
       <c r="C6" t="s">
-        <v>35</v>
+        <v>21</v>
       </c>
       <c r="D6" t="s">
         <v>9</v>
       </c>
       <c r="E6" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F6" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="G6" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="H6" s="5">
-        <v>926.86956521739103</v>
+        <v>24.3913043478261</v>
       </c>
       <c r="I6" s="6">
-        <v>6.4880869565217394E-2</v>
+        <v>1.95130434782609E-2</v>
       </c>
       <c r="J6" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A7" s="1">
-        <v>44846</v>
-      </c>
-      <c r="B7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C7" t="s">
-        <v>35</v>
-      </c>
-      <c r="D7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E7" t="s">
-        <v>15</v>
-      </c>
-      <c r="F7" t="s">
-        <v>16</v>
-      </c>
-      <c r="G7" t="s">
-        <v>26</v>
-      </c>
-      <c r="H7" s="5">
-        <v>73.173913043478294</v>
-      </c>
-      <c r="I7" s="6">
-        <v>2.92695652173913E-2</v>
-      </c>
+      <c r="A7" s="1"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A8" s="1">
-        <v>44846</v>
-      </c>
-      <c r="B8" t="s">
-        <v>8</v>
-      </c>
-      <c r="C8" t="s">
-        <v>36</v>
-      </c>
-      <c r="D8" t="s">
-        <v>9</v>
-      </c>
-      <c r="E8" t="s">
-        <v>10</v>
-      </c>
-      <c r="F8" t="s">
-        <v>11</v>
-      </c>
-      <c r="G8" t="s">
-        <v>28</v>
-      </c>
-      <c r="H8" s="5">
-        <v>97.565217391304301</v>
-      </c>
-      <c r="I8" s="6">
-        <v>1.46347826086957E-2</v>
-      </c>
-      <c r="J8" t="s">
-        <v>12</v>
-      </c>
+      <c r="A8" s="1"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A9" s="1">
-        <v>44846</v>
-      </c>
-      <c r="B9" t="s">
-        <v>8</v>
-      </c>
-      <c r="C9" t="s">
-        <v>36</v>
-      </c>
-      <c r="D9" t="s">
-        <v>9</v>
-      </c>
-      <c r="E9" t="s">
-        <v>13</v>
-      </c>
-      <c r="F9" t="s">
-        <v>14</v>
-      </c>
-      <c r="G9" t="s">
-        <v>27</v>
-      </c>
-      <c r="H9" s="5">
-        <v>414.65217391304299</v>
-      </c>
-      <c r="I9" s="6">
-        <v>6.2197826086956502E-2</v>
-      </c>
-      <c r="J9" t="s">
-        <v>12</v>
-      </c>
+      <c r="A9" s="1"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A10" s="1">
-        <v>44846</v>
-      </c>
-      <c r="B10" t="s">
-        <v>8</v>
-      </c>
-      <c r="C10" t="s">
-        <v>36</v>
-      </c>
-      <c r="D10" t="s">
-        <v>9</v>
-      </c>
-      <c r="E10" t="s">
-        <v>17</v>
-      </c>
-      <c r="F10" t="s">
-        <v>18</v>
-      </c>
-      <c r="G10" t="s">
-        <v>19</v>
-      </c>
-      <c r="H10" s="5">
-        <v>48.7826086956522</v>
-      </c>
-      <c r="I10" s="6">
-        <v>1.9513043478260899E-4</v>
-      </c>
-      <c r="J10" t="s">
-        <v>12</v>
-      </c>
+      <c r="A10" s="1"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A11" s="1">
-        <v>44846</v>
-      </c>
-      <c r="B11" t="s">
-        <v>8</v>
-      </c>
-      <c r="C11" t="s">
-        <v>36</v>
-      </c>
-      <c r="D11" t="s">
-        <v>9</v>
-      </c>
-      <c r="E11" t="s">
-        <v>17</v>
-      </c>
-      <c r="F11" t="s">
-        <v>18</v>
-      </c>
-      <c r="G11" t="s">
-        <v>20</v>
-      </c>
-      <c r="H11" s="5">
-        <v>317.08695652173901</v>
-      </c>
-      <c r="I11" s="6">
-        <v>1.2683478260869601E-3</v>
-      </c>
+      <c r="A11" s="1"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A12" s="1">
-        <v>44846</v>
-      </c>
-      <c r="B12" t="s">
-        <v>8</v>
-      </c>
-      <c r="C12" t="s">
-        <v>36</v>
-      </c>
-      <c r="D12" t="s">
-        <v>9</v>
-      </c>
-      <c r="E12" t="s">
-        <v>17</v>
-      </c>
-      <c r="F12" t="s">
-        <v>18</v>
-      </c>
-      <c r="G12" t="s">
-        <v>21</v>
-      </c>
-      <c r="H12" s="5">
-        <v>2341.5652173912999</v>
-      </c>
-      <c r="I12" s="6">
-        <v>7.0246956521739104E-3</v>
-      </c>
-      <c r="J12" t="s">
-        <v>12</v>
-      </c>
+      <c r="A12" s="1"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A13" s="1">
-        <v>44846</v>
-      </c>
-      <c r="B13" t="s">
-        <v>8</v>
-      </c>
-      <c r="C13" t="s">
-        <v>36</v>
-      </c>
-      <c r="D13" t="s">
-        <v>9</v>
-      </c>
-      <c r="E13" t="s">
-        <v>22</v>
-      </c>
-      <c r="F13" t="s">
-        <v>23</v>
-      </c>
-      <c r="G13" t="s">
-        <v>24</v>
-      </c>
-      <c r="H13" s="5">
-        <v>48.7826086956522</v>
-      </c>
-      <c r="I13" s="6">
-        <v>2.4391304347826099E-3</v>
-      </c>
-      <c r="J13" t="s">
-        <v>12</v>
-      </c>
+      <c r="A13" s="1"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A14" s="1">
-        <v>44846</v>
-      </c>
-      <c r="B14" t="s">
-        <v>8</v>
-      </c>
-      <c r="C14" t="s">
-        <v>36</v>
-      </c>
-      <c r="D14" t="s">
-        <v>9</v>
-      </c>
-      <c r="E14" t="s">
-        <v>15</v>
-      </c>
-      <c r="F14" t="s">
-        <v>16</v>
-      </c>
-      <c r="G14" t="s">
-        <v>25</v>
-      </c>
-      <c r="H14" s="5">
-        <v>48.7826086956522</v>
-      </c>
-      <c r="I14" s="6">
-        <v>9.7565217391304294E-3</v>
-      </c>
-      <c r="J14" t="s">
-        <v>12</v>
-      </c>
+      <c r="A14" s="1"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A15" s="1">
-        <v>44846</v>
-      </c>
-      <c r="B15" t="s">
-        <v>8</v>
-      </c>
-      <c r="C15" t="s">
-        <v>36</v>
-      </c>
-      <c r="D15" t="s">
-        <v>9</v>
-      </c>
-      <c r="E15" t="s">
-        <v>15</v>
-      </c>
-      <c r="F15" t="s">
-        <v>16</v>
-      </c>
-      <c r="G15" t="s">
-        <v>26</v>
-      </c>
-      <c r="H15" s="5">
-        <v>73.173913043478294</v>
-      </c>
-      <c r="I15" s="6">
-        <v>2.92695652173913E-2</v>
-      </c>
+      <c r="A15" s="1"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A16" s="1">
-        <v>44846</v>
-      </c>
-      <c r="B16" t="s">
-        <v>8</v>
-      </c>
-      <c r="C16" t="s">
-        <v>36</v>
-      </c>
-      <c r="D16" t="s">
-        <v>9</v>
-      </c>
-      <c r="E16" t="s">
-        <v>15</v>
-      </c>
-      <c r="F16" t="s">
-        <v>16</v>
-      </c>
-      <c r="G16" t="s">
-        <v>37</v>
-      </c>
-      <c r="H16" s="5">
-        <v>24.3913043478261</v>
-      </c>
-      <c r="I16" s="6">
-        <v>1.95130434782609E-2</v>
-      </c>
-      <c r="J16" t="s">
-        <v>38</v>
-      </c>
+      <c r="A16" s="1"/>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A17" s="1"/>

</xml_diff>